<commit_message>
Implement Upload/Extract Functions For ArcaDigital WebApp
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Codebar_Benki\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176134D1-7D0E-4A68-8051-450D20BCCC12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23159A9-4C1E-47B7-ACB1-4FFFA41252CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="0" windowWidth="27930" windowHeight="15855" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Nombre</t>
   </si>
@@ -105,13 +105,10 @@
     <t>BI001</t>
   </si>
   <si>
-    <t>BILLETERA D&amp;G COLOR NEGRO</t>
-  </si>
-  <si>
     <t>D&amp;G</t>
   </si>
   <si>
-    <t>B1000001</t>
+    <t>Auto Upload Test File</t>
   </si>
 </sst>
 </file>
@@ -171,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,11 +466,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
@@ -555,7 +552,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -597,21 +594,21 @@
         <v>23</v>
       </c>
       <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
         <v>27</v>
       </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
       <c r="Q2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ended Excel Integration New Import Export Web Buttons
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -2,21 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Codebar_Benki\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23159A9-4C1E-47B7-ACB1-4FFFA41252CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2389C3D-2533-4B04-B16B-8252945F92FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="0" windowWidth="27930" windowHeight="15855" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -93,31 +102,19 @@
     <t>PEN</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Gaseosas</t>
-  </si>
-  <si>
-    <t>GA001</t>
-  </si>
-  <si>
-    <t>BI001</t>
-  </si>
-  <si>
-    <t>D&amp;G</t>
-  </si>
-  <si>
-    <t>Auto Upload Test File</t>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SB008-AUTOUPLOAD</t>
+  </si>
+  <si>
+    <t>SB008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,9 +144,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,6 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -552,16 +549,10 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2">
-        <v>51121703</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -570,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>90</v>
+        <v>124.5</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -578,33 +569,20 @@
       <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="J2">
-        <v>70</v>
-      </c>
       <c r="K2">
         <v>10</v>
       </c>
       <c r="L2">
-        <v>4000</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1"/>
       <c r="T2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added bats and Excel EndPoints
</commit_message>
<xml_diff>
--- a/Config/items.xlsx
+++ b/Config/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Codebar_Benki\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2389C3D-2533-4B04-B16B-8252945F92FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA99C466-8E36-4874-BE5D-A5579E2E773C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,10 +105,10 @@
     <t>SI</t>
   </si>
   <si>
-    <t>SB008-AUTOUPLOAD</t>
-  </si>
-  <si>
-    <t>SB008</t>
+    <t>SB009-SECOND</t>
+  </si>
+  <si>
+    <t>SB009</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>124.5</v>
+        <v>55</v>
       </c>
       <c r="H2">
         <v>10</v>

</xml_diff>